<commit_message>
Updated doc and viability calculations
</commit_message>
<xml_diff>
--- a/results/results_table.xlsx
+++ b/results/results_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\anth005\jhu_projects\mol_gan\code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\anth005\jhu_projects\SMGAN\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF4D076-ACE0-49F8-8318-8A75FA2425B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BB6717-73FB-4238-B9E4-C80EC5D5B47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3530CD8D-4535-4D52-9EDB-FADBC0055FB5}"/>
+    <workbookView xWindow="-25290" yWindow="1650" windowWidth="12150" windowHeight="11970" xr2:uid="{3530CD8D-4535-4D52-9EDB-FADBC0055FB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -499,7 +499,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>17.5</v>
+        <v>31.2</v>
       </c>
       <c r="C2" s="7">
         <v>100</v>
@@ -510,10 +510,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="5">
-        <v>2</v>
+        <v>0.05</v>
       </c>
       <c r="C3" s="8">
-        <v>3.2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -532,7 +532,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>0.28000000000000003</v>
+        <v>0.6</v>
       </c>
       <c r="C5" s="8">
         <v>0.89</v>
@@ -543,7 +543,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="C6" s="7">
         <v>0.62</v>
@@ -554,7 +554,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5">
-        <v>0.25</v>
+        <v>0.46</v>
       </c>
       <c r="C7" s="8">
         <v>0.95</v>

</xml_diff>

<commit_message>
Added molecule visualizer and updated ppt
</commit_message>
<xml_diff>
--- a/results/results_table.xlsx
+++ b/results/results_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\anth005\jhu_projects\SMGAN\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BB6717-73FB-4238-B9E4-C80EC5D5B47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEA342B-34C6-4AAB-9705-01B74DA961BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25290" yWindow="1650" windowWidth="12150" windowHeight="11970" xr2:uid="{3530CD8D-4535-4D52-9EDB-FADBC0055FB5}"/>
+    <workbookView xWindow="1035" yWindow="765" windowWidth="21600" windowHeight="11835" xr2:uid="{3530CD8D-4535-4D52-9EDB-FADBC0055FB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Metric</t>
   </si>
@@ -60,7 +60,10 @@
     <t>MolGAN</t>
   </si>
   <si>
-    <t>SMGAN</t>
+    <t>SMGAN BASELINE</t>
+  </si>
+  <si>
+    <t>SMGAN Tuned</t>
   </si>
 </sst>
 </file>
@@ -471,92 +474,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{902EEB00-86C7-4B14-9DAC-4143CD9ADDC8}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
+        <v>17.5</v>
+      </c>
+      <c r="C2" s="3">
         <v>31.2</v>
       </c>
-      <c r="C2" s="7">
+      <c r="D2" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="C3" s="5">
         <v>0.05</v>
       </c>
-      <c r="C3" s="8">
+      <c r="D3" s="8">
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>100</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C5" s="5">
         <v>0.6</v>
       </c>
-      <c r="C5" s="8">
+      <c r="D5" s="8">
         <v>0.89</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="C6" s="3">
         <v>0.02</v>
       </c>
-      <c r="C6" s="7">
+      <c r="D6" s="7">
         <v>0.62</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
+        <v>0.42</v>
+      </c>
+      <c r="C7" s="5">
         <v>0.46</v>
       </c>
-      <c r="C7" s="8">
+      <c r="D7" s="8">
         <v>0.95</v>
       </c>
     </row>

</xml_diff>